<commit_message>
finalised the project so it can now be accessed from aperc github
</commit_message>
<xml_diff>
--- a/input_data/outlook-transport-divisia.xlsx
+++ b/input_data/outlook-transport-divisia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aperc-my.sharepoint.com/personal/finbar_maunsell_aperc_or_jp/Documents/Documents/Github/PyLMDI/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="11_F25DC773A252ABDACC10486A01D871A05BDE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53161DE3-BEC3-4F3F-9737-BA2B779AD599}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="11_F25DC773A252ABDACC10486A01D871A05BDE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E75BBD4C-D5CE-4665-8911-E640F223037A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-6675" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref_pass_energy_pj" sheetId="10" r:id="rId1"/>
@@ -234,6 +234,81 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2238375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3486150</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C88F836-17A3-7078-4B79-A2C5BA213607}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4800600" y="1428750"/>
+          <a:ext cx="6448425" cy="2924175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Not complete!</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,9 +580,9 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -614,7 +689,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -721,7 +796,7 @@
         <v>1098.8749900787225</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -828,7 +903,7 @@
         <v>5166.7537674996374</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -935,7 +1010,7 @@
         <v>1750.1589855637387</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
@@ -1042,7 +1117,7 @@
         <v>7519.6181643449945</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -1149,7 +1224,7 @@
         <v>14718.325966410715</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -1256,7 +1331,7 @@
         <v>492.19682141021468</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -1376,9 +1451,9 @@
       <selection activeCell="F12" sqref="F12:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1485,7 +1560,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -1592,7 +1667,7 @@
         <v>1939.4037047920001</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -1699,7 +1774,7 @@
         <v>3902.3144257569998</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -1806,7 +1881,7 @@
         <v>4107.8885285830002</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
@@ -1913,7 +1988,7 @@
         <v>4180.1916110710008</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -2020,7 +2095,7 @@
         <v>18859.286407203999</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -2127,7 +2202,7 @@
         <v>3425.496389291</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -2247,9 +2322,9 @@
       <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -2356,7 +2431,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -2463,7 +2538,7 @@
         <v>822.32943306718425</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -2570,7 +2645,7 @@
         <v>3814.1790981164095</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -2677,7 +2752,7 @@
         <v>1577.6634404115957</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
@@ -2784,7 +2859,7 @@
         <v>5613.3949035564465</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -2891,7 +2966,7 @@
         <v>7721.7268088613882</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -2998,7 +3073,7 @@
         <v>661.55422446052592</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -3118,9 +3193,9 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -3227,7 +3302,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -3334,7 +3409,7 @@
         <v>1803.7702033640001</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -3441,7 +3516,7 @@
         <v>3397.6694985200002</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -3548,7 +3623,7 @@
         <v>4710.3510365699995</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
@@ -3655,7 +3730,7 @@
         <v>3523.9320517040001</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -3762,7 +3837,7 @@
         <v>16927.088866786999</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -3869,7 +3944,7 @@
         <v>4596.7926291849999</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -3989,9 +4064,9 @@
       <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -4098,7 +4173,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -4205,7 +4280,7 @@
         <v>618.46003401559835</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
@@ -4312,7 +4387,7 @@
         <v>20522.894457881448</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -4419,7 +4494,7 @@
         <v>6272.9690641914549</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -4526,7 +4601,7 @@
         <v>1457.7598547042578</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -4646,9 +4721,9 @@
       <selection activeCell="N36" sqref="N36:N37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -4755,7 +4830,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -4862,7 +4937,7 @@
         <v>94.218745768000005</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
@@ -4969,7 +5044,7 @@
         <v>20852.766053227999</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -5076,7 +5151,7 @@
         <v>1646.008635657</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -5183,7 +5258,7 @@
         <v>11116.465395343001</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -5303,9 +5378,9 @@
       <selection activeCell="D7" sqref="D7:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -5412,7 +5487,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -5519,7 +5594,7 @@
         <v>572.80467161267131</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
@@ -5626,7 +5701,7 @@
         <v>12772.405941909814</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -5733,7 +5808,7 @@
         <v>4476.7471139222616</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -5840,7 +5915,7 @@
         <v>1493.2093156185983</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -5956,13 +6031,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2C1F2F-7766-4EF9-A5EF-412EC5957F16}">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -6069,7 +6144,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -6176,7 +6251,7 @@
         <v>103.06145194600001</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
@@ -6283,7 +6358,7 @@
         <v>16952.352118507999</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -6390,7 +6465,7 @@
         <v>1400.5678301260002</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -6497,7 +6572,7 @@
         <v>12202.253275579002</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -6616,17 +6691,17 @@
   </sheetPr>
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="4" width="74.42578125" customWidth="1"/>
+    <col min="3" max="4" width="74.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -6670,7 +6745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -6680,147 +6755,147 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="5"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="5"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -6828,5 +6903,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>